<commit_message>
fix: update the PUPMMS_Excel.xlsx
</commit_message>
<xml_diff>
--- a/client/public/files/PUPMMS_Excel.xlsx
+++ b/client/public/files/PUPMMS_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Kevin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelisha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A34EB58-EC3A-4144-B1EA-9EFE534ED0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6415320-7E00-45C3-AA0B-06948EB1AF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{35C61CC0-323A-4D09-AF90-824C68199ED7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{35C61CC0-323A-4D09-AF90-824C68199ED7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>address</t>
   </si>
@@ -91,16 +91,117 @@
   </si>
   <si>
     <t>hasNDA</t>
+  </si>
+  <si>
+    <t>Company X</t>
+  </si>
+  <si>
+    <t>Company Y</t>
+  </si>
+  <si>
+    <t>Company Z</t>
+  </si>
+  <si>
+    <t>Practicum</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Information Technology (IT)</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Unit No, Street Name, City</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Dela Cruz</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Reyes</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>IT Head</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>Expired</t>
+  </si>
+  <si>
+    <t>companyx@gmail.com</t>
+  </si>
+  <si>
+    <t>companyy@gmail.com</t>
+  </si>
+  <si>
+    <t>companyz@gmail.com</t>
+  </si>
+  <si>
+    <t>Sta. Mesa, Manila</t>
+  </si>
+  <si>
+    <t>Quezon City</t>
+  </si>
+  <si>
+    <t>Sta. Rosa, Laguna</t>
+  </si>
+  <si>
+    <t>BSCpE</t>
+  </si>
+  <si>
+    <t>BSIT</t>
+  </si>
+  <si>
+    <t>BBTLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,13 +224,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -146,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -292,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -442,28 +547,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720D028C-6EBC-48CF-93F6-58863B73964D}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -525,7 +635,171 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2">
+        <v>12345678910</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2">
+        <v>45316</v>
+      </c>
+      <c r="O2" s="2">
+        <v>46412</v>
+      </c>
+      <c r="P2">
+        <v>2024</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <v>12345678910</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>45395</v>
+      </c>
+      <c r="O3" s="2">
+        <v>45761</v>
+      </c>
+      <c r="P3">
+        <v>2024</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4">
+        <v>12345678910</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>45095</v>
+      </c>
+      <c r="O4" s="2">
+        <v>45461</v>
+      </c>
+      <c r="P4">
+        <v>2023</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{65EA7728-D661-467C-820F-0E687A4C34E4}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{F6DDF2AB-D9ED-49BA-A279-11E4264895E0}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{56FE601B-DAED-48E2-ABE0-EB98467D9B48}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>